<commit_message>
'Add' is getting there but needs tests
</commit_message>
<xml_diff>
--- a/Opcodes.xlsx
+++ b/Opcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newman.c\Source\repos\Z80CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD74B3B4-7C35-428A-BFE7-9015A3DA45CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646AADCD-64FE-47F5-95F0-5247F6ADC421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{048A5853-C2CF-472B-B65B-479DA1D6E657}"/>
+    <workbookView xWindow="32535" yWindow="1020" windowWidth="21600" windowHeight="14205" xr2:uid="{048A5853-C2CF-472B-B65B-479DA1D6E657}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2769,22 +2769,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF609AB8-E8AD-4889-BB06-0C50E76FDAB8}">
-  <dimension ref="A1:D362"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="17" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>691</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>458</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>334</v>
       </c>
@@ -2826,7 +2827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>267</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>205</v>
       </c>
@@ -2854,7 +2855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>204</v>
       </c>
@@ -2868,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>130</v>
       </c>
@@ -2882,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>324</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>568</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>167</v>
       </c>
@@ -2924,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>295</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>131</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>206</v>
       </c>
@@ -2980,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>133</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>342</v>
       </c>
@@ -3008,7 +3009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>589</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>157</v>
       </c>
@@ -3036,7 +3037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>365</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>268</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>209</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>208</v>
       </c>
@@ -3092,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>135</v>
       </c>
@@ -3106,7 +3107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>355</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>559</v>
       </c>
@@ -3134,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>257</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>36</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>297</v>
       </c>
@@ -3176,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>136</v>
       </c>
@@ -3190,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>210</v>
       </c>
@@ -3204,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>138</v>
       </c>
@@ -3218,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>373</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>579</v>
       </c>
@@ -3246,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>263</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>392</v>
       </c>
@@ -3274,7 +3275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>287</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>213</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>212</v>
       </c>
@@ -3316,7 +3317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>140</v>
       </c>
@@ -3330,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>386</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>122</v>
       </c>
@@ -3358,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>265</v>
       </c>
@@ -3372,7 +3373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>37</v>
       </c>
@@ -3386,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>390</v>
       </c>
@@ -3400,7 +3401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>141</v>
       </c>
@@ -3414,7 +3415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>222</v>
       </c>
@@ -3428,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>151</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>426</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>120</v>
       </c>
@@ -3470,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>261</v>
       </c>
@@ -3484,7 +3485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>440</v>
       </c>
@@ -3498,7 +3499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>281</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>224</v>
       </c>
@@ -3526,7 +3527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>197</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>123</v>
       </c>
@@ -3554,7 +3555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>269</v>
       </c>
@@ -3568,7 +3569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>631</v>
       </c>
@@ -3582,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>259</v>
       </c>
@@ -3596,7 +3597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>38</v>
       </c>
@@ -3610,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>305</v>
       </c>
@@ -3624,7 +3625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>153</v>
       </c>
@@ -3638,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>202</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>128</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>307</v>
       </c>
@@ -3680,7 +3681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>95</v>
       </c>
@@ -3694,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>326</v>
       </c>
@@ -3708,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>319</v>
       </c>
@@ -3722,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>344</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>336</v>
       </c>
@@ -3750,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>357</v>
       </c>
@@ -3764,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>350</v>
       </c>
@@ -3778,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>375</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>367</v>
       </c>
@@ -3806,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>388</v>
       </c>
@@ -3820,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>381</v>
       </c>
@@ -3834,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>428</v>
       </c>
@@ -3848,7 +3849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>420</v>
       </c>
@@ -3862,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>271</v>
       </c>
@@ -3876,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>172</v>
       </c>
@@ -3890,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>309</v>
       </c>
@@ -3904,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>299</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>29</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>22</v>
       </c>
@@ -3946,7 +3947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>8</v>
       </c>
@@ -3960,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>0</v>
       </c>
@@ -3974,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>671</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>664</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>617</v>
       </c>
@@ -4016,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>609</v>
       </c>
@@ -4030,7 +4031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>63</v>
       </c>
@@ -4044,7 +4045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>55</v>
       </c>
@@ -4058,7 +4059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>685</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
         <v>677</v>
       </c>
@@ -4086,7 +4087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>467</v>
       </c>
@@ -4100,7 +4101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>459</v>
       </c>
@@ -4114,7 +4115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>105</v>
       </c>
@@ -4128,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>97</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>537</v>
       </c>
@@ -4156,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>499</v>
       </c>
@@ -4170,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>247</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>233</v>
       </c>
@@ -4198,7 +4199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>85</v>
       </c>
@@ -4212,7 +4213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>511</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>27</v>
       </c>
@@ -4240,7 +4241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>593</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>545</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>529</v>
       </c>
@@ -4282,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>255</v>
       </c>
@@ -4296,7 +4297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>566</v>
       </c>
@@ -4310,7 +4311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>560</v>
       </c>
@@ -4324,7 +4325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>587</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>581</v>
       </c>
@@ -4352,7 +4353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>557</v>
       </c>
@@ -4366,7 +4367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>551</v>
       </c>
@@ -4380,7 +4381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>577</v>
       </c>
@@ -4394,7 +4395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>571</v>
       </c>
@@ -4408,7 +4409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>646</v>
       </c>
@@ -4422,7 +4423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>640</v>
       </c>
@@ -4436,7 +4437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>654</v>
       </c>
@@ -4450,7 +4451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>648</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>662</v>
       </c>
@@ -4478,7 +4479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>656</v>
       </c>
@@ -4492,7 +4493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>75</v>
       </c>
@@ -4506,7 +4507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>69</v>
       </c>
@@ -4520,7 +4521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>527</v>
       </c>
@@ -4534,7 +4535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>521</v>
       </c>
@@ -4548,7 +4549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>638</v>
       </c>
@@ -4562,7 +4563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>632</v>
       </c>
@@ -4576,7 +4577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>93</v>
       </c>
@@ -4590,7 +4591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>77</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>6</v>
       </c>
@@ -4618,7 +4619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>595</v>
       </c>
@@ -4632,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>535</v>
       </c>
@@ -4646,7 +4647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>501</v>
       </c>
@@ -4660,7 +4661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>245</v>
       </c>
@@ -4674,7 +4675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>491</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
         <v>83</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
         <v>513</v>
       </c>
@@ -4716,7 +4717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
         <v>669</v>
       </c>
@@ -4730,7 +4731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
         <v>597</v>
       </c>
@@ -4744,7 +4745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
         <v>531</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>170</v>
       </c>
@@ -4772,7 +4773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>241</v>
       </c>
@@ -4786,7 +4787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>181</v>
       </c>
@@ -4800,7 +4801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
         <v>79</v>
       </c>
@@ -4814,7 +4815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
         <v>218</v>
       </c>
@@ -4828,7 +4829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
         <v>147</v>
       </c>
@@ -4842,7 +4843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
         <v>39</v>
       </c>
@@ -4856,7 +4857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="6" t="s">
         <v>41</v>
       </c>
@@ -4870,7 +4871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6" t="s">
         <v>398</v>
       </c>
@@ -4884,7 +4885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="6" t="s">
         <v>289</v>
       </c>
@@ -4898,7 +4899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>214</v>
       </c>
@@ -4912,7 +4913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="6" t="s">
         <v>400</v>
       </c>
@@ -4926,7 +4927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="6" t="s">
         <v>43</v>
       </c>
@@ -4940,7 +4941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="6" t="s">
         <v>396</v>
       </c>
@@ -4954,7 +4955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="6" t="s">
         <v>143</v>
       </c>
@@ -4968,7 +4969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
         <v>404</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>198</v>
       </c>
@@ -4996,7 +4997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>124</v>
       </c>
@@ -5010,7 +5011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>273</v>
       </c>
@@ -5024,7 +5025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="6" t="s">
         <v>45</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="6" t="s">
         <v>328</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="6" t="s">
         <v>320</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="6" t="s">
         <v>346</v>
       </c>
@@ -5080,7 +5081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="6" t="s">
         <v>338</v>
       </c>
@@ -5094,7 +5095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="6" t="s">
         <v>359</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>351</v>
       </c>
@@ -5122,7 +5123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>377</v>
       </c>
@@ -5136,7 +5137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="6" t="s">
         <v>369</v>
       </c>
@@ -5150,7 +5151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="6" t="s">
         <v>402</v>
       </c>
@@ -5164,7 +5165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="6" t="s">
         <v>382</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
         <v>406</v>
       </c>
@@ -5192,7 +5193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>422</v>
       </c>
@@ -5206,7 +5207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>275</v>
       </c>
@@ -5220,7 +5221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>311</v>
       </c>
@@ -5234,7 +5235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>301</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
         <v>31</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>23</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
         <v>10</v>
       </c>
@@ -5290,7 +5291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="6" t="s">
         <v>2</v>
       </c>
@@ -5304,7 +5305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
         <v>673</v>
       </c>
@@ -5318,7 +5319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>665</v>
       </c>
@@ -5332,7 +5333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>619</v>
       </c>
@@ -5346,7 +5347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>611</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
         <v>65</v>
       </c>
@@ -5374,7 +5375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
         <v>57</v>
       </c>
@@ -5388,7 +5389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
         <v>687</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
         <v>679</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
         <v>469</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="6" t="s">
         <v>461</v>
       </c>
@@ -5444,7 +5445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
         <v>107</v>
       </c>
@@ -5458,7 +5459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>99</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>562</v>
       </c>
@@ -5486,7 +5487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
         <v>583</v>
       </c>
@@ -5500,7 +5501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
         <v>553</v>
       </c>
@@ -5514,7 +5515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
         <v>573</v>
       </c>
@@ -5528,7 +5529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
         <v>642</v>
       </c>
@@ -5542,7 +5543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>650</v>
       </c>
@@ -5556,7 +5557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
         <v>658</v>
       </c>
@@ -5570,7 +5571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
         <v>71</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="6" t="s">
         <v>523</v>
       </c>
@@ -5598,7 +5599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
         <v>634</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
         <v>505</v>
       </c>
@@ -5626,7 +5627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
         <v>163</v>
       </c>
@@ -5640,7 +5641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
         <v>517</v>
       </c>
@@ -5654,7 +5655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
         <v>237</v>
       </c>
@@ -5668,7 +5669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="6" t="s">
         <v>436</v>
       </c>
@@ -5682,7 +5683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="6" t="s">
         <v>615</v>
       </c>
@@ -5696,7 +5697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="6" t="s">
         <v>599</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
         <v>543</v>
       </c>
@@ -5724,7 +5725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="6" t="s">
         <v>503</v>
       </c>
@@ -5738,7 +5739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="6" t="s">
         <v>253</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="6" t="s">
         <v>161</v>
       </c>
@@ -5766,7 +5767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="6" t="s">
         <v>91</v>
       </c>
@@ -5780,7 +5781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="6" t="s">
         <v>515</v>
       </c>
@@ -5794,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="6" t="s">
         <v>61</v>
       </c>
@@ -5808,7 +5809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="6" t="s">
         <v>601</v>
       </c>
@@ -5822,7 +5823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="6" t="s">
         <v>541</v>
       </c>
@@ -5836,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="6" t="s">
         <v>235</v>
       </c>
@@ -5850,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="6" t="s">
         <v>251</v>
       </c>
@@ -5864,7 +5865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="6" t="s">
         <v>168</v>
       </c>
@@ -5878,7 +5879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="6" t="s">
         <v>89</v>
       </c>
@@ -5892,7 +5893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6" t="s">
         <v>183</v>
       </c>
@@ -5906,7 +5907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="6" t="s">
         <v>479</v>
       </c>
@@ -5920,7 +5921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="6" t="s">
         <v>623</v>
       </c>
@@ -5934,7 +5935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="6" t="s">
         <v>283</v>
       </c>
@@ -5948,7 +5949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="6" t="s">
         <v>456</v>
       </c>
@@ -5962,7 +5963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="6" t="s">
         <v>549</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6" t="s">
         <v>173</v>
       </c>
@@ -5990,7 +5991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="6" t="s">
         <v>394</v>
       </c>
@@ -6004,7 +6005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="6" t="s">
         <v>185</v>
       </c>
@@ -6018,7 +6019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="6" t="s">
         <v>481</v>
       </c>
@@ -6032,7 +6033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="6" t="s">
         <v>14</v>
       </c>
@@ -6046,7 +6047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
         <v>332</v>
       </c>
@@ -6060,7 +6061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
         <v>547</v>
       </c>
@@ -6074,7 +6075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="6" t="s">
         <v>430</v>
       </c>
@@ -6088,7 +6089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6" t="s">
         <v>187</v>
       </c>
@@ -6102,7 +6103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6" t="s">
         <v>483</v>
       </c>
@@ -6116,7 +6117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="6" t="s">
         <v>625</v>
       </c>
@@ -6130,7 +6131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="6" t="s">
         <v>285</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="6" t="s">
         <v>175</v>
       </c>
@@ -6158,7 +6159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="6" t="s">
         <v>315</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="6" t="s">
         <v>189</v>
       </c>
@@ -6186,7 +6187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="6" t="s">
         <v>485</v>
       </c>
@@ -6200,7 +6201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="6" t="s">
         <v>16</v>
       </c>
@@ -6214,7 +6215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
         <v>363</v>
       </c>
@@ -6228,7 +6229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="6" t="s">
         <v>177</v>
       </c>
@@ -6242,7 +6243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="6" t="s">
         <v>317</v>
       </c>
@@ -6256,7 +6257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="6" t="s">
         <v>191</v>
       </c>
@@ -6270,7 +6271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="6" t="s">
         <v>487</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="6" t="s">
         <v>627</v>
       </c>
@@ -6298,7 +6299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="6" t="s">
         <v>591</v>
       </c>
@@ -6312,7 +6313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="6" t="s">
         <v>193</v>
       </c>
@@ -6326,7 +6327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="6" t="s">
         <v>489</v>
       </c>
@@ -6340,7 +6341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6" t="s">
         <v>18</v>
       </c>
@@ -6354,7 +6355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="6" t="s">
         <v>569</v>
       </c>
@@ -6368,7 +6369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="6" t="s">
         <v>195</v>
       </c>
@@ -6382,7 +6383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="6" t="s">
         <v>629</v>
       </c>
@@ -6396,7 +6397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="6" t="s">
         <v>293</v>
       </c>
@@ -6410,7 +6411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="6" t="s">
         <v>179</v>
       </c>
@@ -6424,7 +6425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6" t="s">
         <v>477</v>
       </c>
@@ -6438,7 +6439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="6" t="s">
         <v>20</v>
       </c>
@@ -6452,7 +6453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="6" t="s">
         <v>432</v>
       </c>
@@ -6466,7 +6467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6" t="s">
         <v>446</v>
       </c>
@@ -6480,7 +6481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="6" t="s">
         <v>116</v>
       </c>
@@ -6494,7 +6495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="6" t="s">
         <v>229</v>
       </c>
@@ -6508,7 +6509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="6" t="s">
         <v>495</v>
       </c>
@@ -6522,7 +6523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="6" t="s">
         <v>442</v>
       </c>
@@ -6536,7 +6537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="6" t="s">
         <v>111</v>
       </c>
@@ -6550,7 +6551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6" t="s">
         <v>225</v>
       </c>
@@ -6564,7 +6565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="6" t="s">
         <v>493</v>
       </c>
@@ -6578,7 +6579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="6" t="s">
         <v>448</v>
       </c>
@@ -6592,7 +6593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="6" t="s">
         <v>118</v>
       </c>
@@ -6606,7 +6607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="6" t="s">
         <v>231</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="6" t="s">
         <v>475</v>
       </c>
@@ -6634,7 +6635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6" t="s">
         <v>444</v>
       </c>
@@ -6648,7 +6649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6" t="s">
         <v>113</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6" t="s">
         <v>227</v>
       </c>
@@ -6676,7 +6677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6" t="s">
         <v>473</v>
       </c>
@@ -6690,7 +6691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6" t="s">
         <v>450</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6" t="s">
         <v>452</v>
       </c>
@@ -6714,7 +6715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6" t="s">
         <v>454</v>
       </c>
@@ -6726,7 +6727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6" t="s">
         <v>683</v>
       </c>
@@ -6740,7 +6741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6" t="s">
         <v>603</v>
       </c>
@@ -6754,7 +6755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6" t="s">
         <v>539</v>
       </c>
@@ -6768,7 +6769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6" t="s">
         <v>497</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6" t="s">
         <v>249</v>
       </c>
@@ -6796,7 +6797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6" t="s">
         <v>155</v>
       </c>
@@ -6810,7 +6811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="6" t="s">
         <v>87</v>
       </c>
@@ -6824,7 +6825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="6" t="s">
         <v>509</v>
       </c>
@@ -6838,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="6" t="s">
         <v>465</v>
       </c>
@@ -6852,7 +6853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="6" t="s">
         <v>605</v>
       </c>
@@ -6866,7 +6867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="6" t="s">
         <v>533</v>
       </c>
@@ -6880,7 +6881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="6" t="s">
         <v>434</v>
       </c>
@@ -6894,7 +6895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="6" t="s">
         <v>243</v>
       </c>
@@ -6908,7 +6909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="6" t="s">
         <v>159</v>
       </c>
@@ -6922,7 +6923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="6" t="s">
         <v>81</v>
       </c>
@@ -6936,7 +6937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="6" t="s">
         <v>220</v>
       </c>
@@ -6950,7 +6951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="6" t="s">
         <v>149</v>
       </c>
@@ -6964,7 +6965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A300" s="6" t="s">
         <v>47</v>
       </c>
@@ -6978,7 +6979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A301" s="6" t="s">
         <v>49</v>
       </c>
@@ -6992,7 +6993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="6" t="s">
         <v>410</v>
       </c>
@@ -7006,7 +7007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="6" t="s">
         <v>291</v>
       </c>
@@ -7020,7 +7021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="6" t="s">
         <v>216</v>
       </c>
@@ -7034,7 +7035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="6" t="s">
         <v>412</v>
       </c>
@@ -7048,7 +7049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="6" t="s">
         <v>51</v>
       </c>
@@ -7062,7 +7063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="6" t="s">
         <v>408</v>
       </c>
@@ -7076,7 +7077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="6" t="s">
         <v>145</v>
       </c>
@@ -7090,7 +7091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="6" t="s">
         <v>416</v>
       </c>
@@ -7104,7 +7105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="6" t="s">
         <v>200</v>
       </c>
@@ -7118,7 +7119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A311" s="6" t="s">
         <v>126</v>
       </c>
@@ -7132,7 +7133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="6" t="s">
         <v>277</v>
       </c>
@@ -7146,7 +7147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="6" t="s">
         <v>53</v>
       </c>
@@ -7160,7 +7161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="6" t="s">
         <v>330</v>
       </c>
@@ -7174,7 +7175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="6" t="s">
         <v>322</v>
       </c>
@@ -7188,7 +7189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="6" t="s">
         <v>348</v>
       </c>
@@ -7202,7 +7203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="6" t="s">
         <v>340</v>
       </c>
@@ -7216,7 +7217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="6" t="s">
         <v>361</v>
       </c>
@@ -7230,7 +7231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A319" s="6" t="s">
         <v>353</v>
       </c>
@@ -7244,7 +7245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A320" s="6" t="s">
         <v>379</v>
       </c>
@@ -7258,7 +7259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="6" t="s">
         <v>371</v>
       </c>
@@ -7272,7 +7273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="6" t="s">
         <v>414</v>
       </c>
@@ -7286,7 +7287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="6" t="s">
         <v>384</v>
       </c>
@@ -7300,7 +7301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="6" t="s">
         <v>418</v>
       </c>
@@ -7314,7 +7315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A325" s="6" t="s">
         <v>424</v>
       </c>
@@ -7328,7 +7329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="326" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="6" t="s">
         <v>279</v>
       </c>
@@ -7342,7 +7343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A327" s="6" t="s">
         <v>313</v>
       </c>
@@ -7356,7 +7357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="6" t="s">
         <v>303</v>
       </c>
@@ -7370,7 +7371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="6" t="s">
         <v>33</v>
       </c>
@@ -7384,7 +7385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="6" t="s">
         <v>25</v>
       </c>
@@ -7398,7 +7399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="331" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="6" t="s">
         <v>12</v>
       </c>
@@ -7412,7 +7413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A332" s="6" t="s">
         <v>4</v>
       </c>
@@ -7426,7 +7427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="333" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="6" t="s">
         <v>675</v>
       </c>
@@ -7440,7 +7441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="6" t="s">
         <v>667</v>
       </c>
@@ -7454,7 +7455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="6" t="s">
         <v>621</v>
       </c>
@@ -7468,7 +7469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="6" t="s">
         <v>613</v>
       </c>
@@ -7482,7 +7483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="337" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="6" t="s">
         <v>67</v>
       </c>
@@ -7496,7 +7497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338" s="6" t="s">
         <v>59</v>
       </c>
@@ -7510,7 +7511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A339" s="6" t="s">
         <v>689</v>
       </c>
@@ -7524,7 +7525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" s="6" t="s">
         <v>681</v>
       </c>
@@ -7538,7 +7539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="6" t="s">
         <v>471</v>
       </c>
@@ -7552,7 +7553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="342" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A342" s="6" t="s">
         <v>463</v>
       </c>
@@ -7566,7 +7567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A343" s="6" t="s">
         <v>109</v>
       </c>
@@ -7580,7 +7581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A344" s="6" t="s">
         <v>101</v>
       </c>
@@ -7594,7 +7595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="6" t="s">
         <v>564</v>
       </c>
@@ -7608,7 +7609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A346" s="6" t="s">
         <v>585</v>
       </c>
@@ -7622,7 +7623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="6" t="s">
         <v>555</v>
       </c>
@@ -7636,7 +7637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="348" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348" s="6" t="s">
         <v>575</v>
       </c>
@@ -7650,7 +7651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="6" t="s">
         <v>644</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A350" s="6" t="s">
         <v>652</v>
       </c>
@@ -7678,7 +7679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="351" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A351" s="6" t="s">
         <v>660</v>
       </c>
@@ -7692,7 +7693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="6" t="s">
         <v>73</v>
       </c>
@@ -7706,7 +7707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" s="6" t="s">
         <v>525</v>
       </c>
@@ -7720,7 +7721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="354" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" s="6" t="s">
         <v>636</v>
       </c>
@@ -7734,7 +7735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="355" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" s="6" t="s">
         <v>507</v>
       </c>
@@ -7748,7 +7749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="356" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="6" t="s">
         <v>165</v>
       </c>
@@ -7762,7 +7763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="357" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="6" t="s">
         <v>519</v>
       </c>
@@ -7776,7 +7777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358" s="6" t="s">
         <v>239</v>
       </c>
@@ -7790,7 +7791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="6" t="s">
         <v>438</v>
       </c>
@@ -7804,7 +7805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="6" t="s">
         <v>103</v>
       </c>
@@ -7818,7 +7819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="361" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="8" t="s">
         <v>607</v>
       </c>
@@ -7832,9 +7833,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:D361" xr:uid="{88676A4B-8439-4FF1-B4AC-A0095F178336}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D361">
       <sortCondition ref="C1:C361"/>
     </sortState>

</xml_diff>